<commit_message>
summary block heading is writing
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>Test title</t>
   </si>
@@ -28,55 +28,82 @@
     <t>(-0.001, 25.0]</t>
   </si>
   <si>
+    <t>(25.0, 45.0]</t>
+  </si>
+  <si>
+    <t>(45.0, 65.0]</t>
+  </si>
+  <si>
+    <t>(65.0, 100.0]</t>
+  </si>
+  <si>
+    <t>preference_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> are more curious to try Soap flavored Bertie Bott's Every Flavour Beans than Earthworm flavored Bertie Bott's Every Flavour Beans</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> believe climate change is a serious threat to human survival</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> believe it should be legal to use psychedelic drugs  (e.g. LSD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can juggle with 3 balls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> own crypto currency (e.g. Bitcoin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prefer red over blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would feel safer in a self-driving car (rather than driving themselves)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would prefer Dick Cheney over Sarah Palin to be president of the United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would rather have the superpower of flight than super strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would rather spend their evening going to a play at the theater than seeing a movie</t>
+  </si>
+  <si>
+    <t>Pooled</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>sum1</t>
+  </si>
+  <si>
+    <t>Truth</t>
+  </si>
+  <si>
+    <t>sum2</t>
+  </si>
+  <si>
+    <t>SecondEstBetter</t>
+  </si>
+  <si>
+    <t>SecondEst</t>
+  </si>
+  <si>
+    <t>SecondEstBetter = 0</t>
+  </si>
+  <si>
+    <t>(25.0, 50.0]</t>
+  </si>
+  <si>
+    <t>(50.0, 65.0]</t>
+  </si>
+  <si>
     <t>(25.0, 47.0]</t>
   </si>
   <si>
     <t>(47.0, 65.0]</t>
-  </si>
-  <si>
-    <t>(65.0, 100.0]</t>
-  </si>
-  <si>
-    <t>preference_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> are more curious to try Soap flavored Bertie Bott's Every Flavour Beans than Earthworm flavored Bertie Bott's Every Flavour Beans</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> believe climate change is a serious threat to human survival</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> believe it should be legal to use psychedelic drugs  (e.g. LSD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> can juggle with 3 balls</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> own crypto currency (e.g. Bitcoin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> prefer red over blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> would feel safer in a self-driving car (rather than driving themselves)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> would prefer Dick Cheney over Sarah Palin to be president of the United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> would rather have the superpower of flight than super strength</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> would rather spend their evening going to a play at the theater than seeing a movie</t>
-  </si>
-  <si>
-    <t>Pooled</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>SecondEstBetter = 0</t>
   </si>
 </sst>
 </file>
@@ -425,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -463,339 +490,402 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="3" t="s">
+    <row r="24" spans="1:11">
+      <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="B25" s="1" t="s">
+    <row r="27" spans="1:11">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="B26" s="1" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="B29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="2" t="s">
+      <c r="C29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="3" t="s">
+    <row r="32" spans="1:11">
+      <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="2" t="s">
-        <v>7</v>
+      <c r="A33" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="3" t="s">
-        <v>11</v>
+      <c r="A37" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="2" t="s">
-        <v>18</v>
+      <c r="A45" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="B49" s="1" t="s">
+    <row r="53" spans="1:11">
+      <c r="B53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="B50" s="1" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="B54" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="3" t="s">
-        <v>6</v>
+      <c r="B55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="B56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="3" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="3" t="s">
-        <v>13</v>
+      <c r="A63" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="2" t="s">
-        <v>18</v>
+      <c r="A69" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B25:K25"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B49:K49"/>
-    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B53:K53"/>
+    <mergeCell ref="B54:K54"/>
+    <mergeCell ref="C55:D55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
need to redo dataframe
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,21 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Pooled</t>
   </si>
   <si>
+    <t>First Estimate</t>
+  </si>
+  <si>
+    <t>(-0.001, 25.0]</t>
+  </si>
+  <si>
+    <t>(25.0, 47.0]</t>
+  </si>
+  <si>
+    <t>(47.0, 65.0]</t>
+  </si>
+  <si>
+    <t>(65.0, 100.0]</t>
+  </si>
+  <si>
+    <t>Preference question</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> are more curious to try Soap flavored Bertie Bott's Every Flavour Beans than Earthworm flavored Bertie Bott's Every Flavour Beans</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> believe climate change is a serious threat to human survival</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> believe it should be legal to use psychedelic drugs  (e.g. LSD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can juggle with 3 balls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> own crypto currency (e.g. Bitcoin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prefer red over blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would feel safer in a self-driving car (rather than driving themselves)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would prefer Dick Cheney over Sarah Palin to be president of the United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would rather have the superpower of flight than super strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> would rather spend their evening going to a play at the theater than seeing a movie</t>
+  </si>
+  <si>
     <t>---</t>
   </si>
   <si>
     <t>Summary Statistics</t>
   </si>
   <si>
-    <t>SecondEst</t>
-  </si>
-  <si>
-    <t>SecondEstBetter</t>
+    <t>Second Estimate</t>
+  </si>
+  <si>
+    <t>% of Time Second Estimate is Preferred to First Estimate</t>
   </si>
   <si>
     <t>45.82 
@@ -397,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,32 +466,196 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>